<commit_message>
GK: add Palestinians to the taz to fix bug- students and emp (current)
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/okev_factor.xlsx
+++ b/create_forecast_basic/current/Intermediates/okev_factor.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
GK: emp current create end of forecast before adding geo info
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/okev_factor.xlsx
+++ b/create_forecast_basic/current/Intermediates/okev_factor.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.481</v>
+        <v>0.455</v>
       </c>
       <c r="C2" t="n">
-        <v>0.631</v>
+        <v>0.605</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.331</v>
+        <v>0.305</v>
       </c>
       <c r="C3" t="n">
-        <v>0.481</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.181</v>
+        <v>0.155</v>
       </c>
       <c r="C4" t="n">
-        <v>0.331</v>
+        <v>0.305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GK: emp_current_year dis emp not okev with v3 pre fix bug
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/Intermediates/okev_factor.xlsx
+++ b/create_forecast_basic/current/Intermediates/okev_factor.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.455</v>
+        <v>0.451</v>
       </c>
       <c r="C2" t="n">
-        <v>0.605</v>
+        <v>0.601</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.305</v>
+        <v>0.301</v>
       </c>
       <c r="C3" t="n">
-        <v>0.455</v>
+        <v>0.451</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.155</v>
+        <v>0.151</v>
       </c>
       <c r="C4" t="n">
-        <v>0.305</v>
+        <v>0.301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>